<commit_message>
Update report-checklist and data.json
commonName auth : A1#111DEDALUS0000
subject_application_vendor : Dedalus
subject_application_id : 4C Suite
subject_application_version : 6.4
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111DEDALUS0000/DEDALUS/4C_Suite/6.4/report-checklist.xlsx
+++ b/GATEWAY/A1#111DEDALUS0000/DEDALUS/4C_Suite/6.4/report-checklist.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\enrico.badolati\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\enrico.badolati\OneDrive - Dedalus S.p.A\Documenti\FSE2.0\test\DEDALUS\4C_Suite\6.4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B111FC32-CA5F-4809-8C61-F50BE966B6E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7156B22-0A1D-47D0-8408-81B3B06B670B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23148" yWindow="-828" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Istruzioni Compilazione" sheetId="1" r:id="rId1"/>
@@ -835,15 +835,6 @@
 </t>
   </si>
   <si>
-    <t>2024-09-26T10:28:21</t>
-  </si>
-  <si>
-    <t>2024-09-26T07:08:44</t>
-  </si>
-  <si>
-    <t>2024-09-26T106:36:41</t>
-  </si>
-  <si>
     <t>2024-09-26T06:38:06</t>
   </si>
   <si>
@@ -877,12 +868,6 @@
     <t>2024-09-26T06:49:55</t>
   </si>
   <si>
-    <t>2024-09-26T09:27:29</t>
-  </si>
-  <si>
-    <t>2024-09-26T09:29:30</t>
-  </si>
-  <si>
     <t>2024-09-26T07:23:22</t>
   </si>
   <si>
@@ -928,12 +913,6 @@
     <t>2024-09-26T07:24:38</t>
   </si>
   <si>
-    <t>580f6419818727ab</t>
-  </si>
-  <si>
-    <t>c5b1c4890bb742de</t>
-  </si>
-  <si>
     <t>f437356a83892d4a</t>
   </si>
   <si>
@@ -967,12 +946,6 @@
     <t>f1da3250624e45df</t>
   </si>
   <si>
-    <t>ff473e48b4dcd130</t>
-  </si>
-  <si>
-    <t>dc92e7d1e3a746a9</t>
-  </si>
-  <si>
     <t>7020c24e453b5f0d</t>
   </si>
   <si>
@@ -1018,12 +991,6 @@
     <t>b7ad5c36be995b5a</t>
   </si>
   <si>
-    <t>2.16.840.1.113883.2.9.2.120103.4.4.1097da1b7bb1f261ff64358ab1435f457c303590a64deffe2cceb322520901ed.5dc60ecfd6^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120103.4.4.6a51afd6dba6889e3eafb79d8198217e9d46d2eeb27bfda1ae52d55a2e4506e8.72d40c24b2^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>UNKNOWN_WORKFLOW_ID</t>
   </si>
   <si>
@@ -1097,12 +1064,6 @@
   </si>
   <si>
     <t>2.16.840.1.113883.2.9.2.120103.4.4.d7b0ac4bd81058ada7ed526c7dc7fe5ca60b6b3e977964fb3a8f0e10cad178e8.718bc80b7b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>5924dc3c392f39ad</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120103.4.4.524da43d04975eefc9278377dbf86cdc13925be8aa313ec7ec6d58c1b3d84538.2f9972dc6b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>"Campo token JWT non valido: Il campo purpose_of_use non è valorizzato"</t>
@@ -1204,6 +1165,45 @@
   </si>
   <si>
     <t>Dedalus S.p.A.</t>
+  </si>
+  <si>
+    <t>128537f2240b4b57</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120103.4.4.6a51afd6dba6889e3eafb79d8198217e9d46d2eeb27bfda1ae52d55a2e4506e8.54261cbc1d^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2024-10-21T107:31:40</t>
+  </si>
+  <si>
+    <t>2024-10-21T07:37:07</t>
+  </si>
+  <si>
+    <t>3b583aedc42dfef0</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120103.4.4.1097da1b7bb1f261ff64358ab1435f457c303590a64deffe2cceb322520901ed.c7db03aaca^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>662e2e9018473b85</t>
+  </si>
+  <si>
+    <t>2024-10-21T07:47:41</t>
+  </si>
+  <si>
+    <t>2024-10-21T07:50:02</t>
+  </si>
+  <si>
+    <t>306733df9ec6bb62</t>
+  </si>
+  <si>
+    <t>2024-10-21T07:54:38</t>
+  </si>
+  <si>
+    <t>44c4d30b28ca8506</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120103.4.4.524da43d04975eefc9278377dbf86cdc13925be8aa313ec7ec6d58c1b3d84538.d9a634876f^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
 </sst>
 </file>
@@ -3340,10 +3340,10 @@
   <dimension ref="A1:W640"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="B20" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="E48" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="F14" sqref="F14"/>
+      <selection pane="bottomRight" activeCell="F56" sqref="F56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -3395,7 +3395,7 @@
       </c>
       <c r="B2" s="47"/>
       <c r="C2" s="48" t="s">
-        <v>306</v>
+        <v>293</v>
       </c>
       <c r="D2" s="47"/>
       <c r="F2" s="6"/>
@@ -3423,7 +3423,7 @@
       </c>
       <c r="B3" s="50"/>
       <c r="C3" s="55" t="s">
-        <v>303</v>
+        <v>290</v>
       </c>
       <c r="D3" s="47"/>
       <c r="F3" s="6"/>
@@ -3449,7 +3449,7 @@
       <c r="A4" s="51"/>
       <c r="B4" s="52"/>
       <c r="C4" s="55" t="s">
-        <v>305</v>
+        <v>292</v>
       </c>
       <c r="D4" s="47"/>
       <c r="E4" s="4"/>
@@ -3476,7 +3476,7 @@
       <c r="A5" s="53"/>
       <c r="B5" s="54"/>
       <c r="C5" s="55" t="s">
-        <v>304</v>
+        <v>291</v>
       </c>
       <c r="D5" s="47"/>
       <c r="F5" s="6"/>
@@ -3652,16 +3652,16 @@
         <v>155</v>
       </c>
       <c r="F10" s="31">
-        <v>45561</v>
+        <v>45586</v>
       </c>
       <c r="G10" s="32" t="s">
-        <v>186</v>
+        <v>296</v>
       </c>
       <c r="H10" s="32" t="s">
-        <v>216</v>
+        <v>294</v>
       </c>
       <c r="I10" s="32" t="s">
-        <v>246</v>
+        <v>295</v>
       </c>
       <c r="J10" s="33" t="s">
         <v>55</v>
@@ -3700,7 +3700,9 @@
       <c r="E11" s="30" t="s">
         <v>156</v>
       </c>
-      <c r="F11" s="31"/>
+      <c r="F11" s="31">
+        <v>45561</v>
+      </c>
       <c r="G11" s="32"/>
       <c r="H11" s="32"/>
       <c r="I11" s="32"/>
@@ -3741,7 +3743,9 @@
       <c r="E12" s="30" t="s">
         <v>157</v>
       </c>
-      <c r="F12" s="31"/>
+      <c r="F12" s="31">
+        <v>45561</v>
+      </c>
       <c r="G12" s="32"/>
       <c r="H12" s="32"/>
       <c r="I12" s="32"/>
@@ -3782,7 +3786,9 @@
       <c r="E13" s="30" t="s">
         <v>158</v>
       </c>
-      <c r="F13" s="31"/>
+      <c r="F13" s="31">
+        <v>45561</v>
+      </c>
       <c r="G13" s="32"/>
       <c r="H13" s="32"/>
       <c r="I13" s="32"/>
@@ -3827,13 +3833,13 @@
         <v>45561</v>
       </c>
       <c r="G14" s="32" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="H14" s="32" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
       <c r="I14" s="32" t="s">
-        <v>247</v>
+        <v>236</v>
       </c>
       <c r="J14" s="33" t="s">
         <v>55</v>
@@ -3847,7 +3853,7 @@
         <v>55</v>
       </c>
       <c r="O14" s="33" t="s">
-        <v>274</v>
+        <v>261</v>
       </c>
       <c r="P14" s="33" t="s">
         <v>55</v>
@@ -3859,7 +3865,7 @@
         <v>55</v>
       </c>
       <c r="S14" s="33" t="s">
-        <v>285</v>
+        <v>272</v>
       </c>
       <c r="T14" s="33" t="s">
         <v>118</v>
@@ -3887,16 +3893,16 @@
         <v>46</v>
       </c>
       <c r="F15" s="31">
-        <v>45561</v>
+        <v>45586</v>
       </c>
       <c r="G15" s="32" t="s">
-        <v>198</v>
+        <v>301</v>
       </c>
       <c r="H15" s="32" t="s">
-        <v>228</v>
+        <v>300</v>
       </c>
       <c r="I15" s="32" t="s">
-        <v>247</v>
+        <v>236</v>
       </c>
       <c r="J15" s="33" t="s">
         <v>55</v>
@@ -3909,7 +3915,7 @@
         <v>55</v>
       </c>
       <c r="O15" s="33" t="s">
-        <v>274</v>
+        <v>261</v>
       </c>
       <c r="P15" s="33" t="s">
         <v>55</v>
@@ -3921,7 +3927,7 @@
         <v>55</v>
       </c>
       <c r="S15" s="33" t="s">
-        <v>286</v>
+        <v>273</v>
       </c>
       <c r="T15" s="33" t="s">
         <v>118</v>
@@ -3952,13 +3958,13 @@
         <v>45561</v>
       </c>
       <c r="G16" s="32" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="H16" s="32" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
       <c r="I16" s="32" t="s">
-        <v>247</v>
+        <v>236</v>
       </c>
       <c r="J16" s="33" t="s">
         <v>55</v>
@@ -3972,7 +3978,7 @@
         <v>55</v>
       </c>
       <c r="O16" s="33" t="s">
-        <v>275</v>
+        <v>262</v>
       </c>
       <c r="P16" s="33" t="s">
         <v>55</v>
@@ -3984,7 +3990,7 @@
         <v>55</v>
       </c>
       <c r="S16" s="33" t="s">
-        <v>286</v>
+        <v>273</v>
       </c>
       <c r="T16" s="33" t="s">
         <v>118</v>
@@ -4012,16 +4018,16 @@
         <v>52</v>
       </c>
       <c r="F17" s="31">
-        <v>45561</v>
+        <v>45586</v>
       </c>
       <c r="G17" s="32" t="s">
-        <v>199</v>
+        <v>302</v>
       </c>
       <c r="H17" s="32" t="s">
-        <v>229</v>
+        <v>303</v>
       </c>
       <c r="I17" s="32" t="s">
-        <v>247</v>
+        <v>236</v>
       </c>
       <c r="J17" s="33" t="s">
         <v>55</v>
@@ -4035,7 +4041,7 @@
         <v>55</v>
       </c>
       <c r="O17" s="33" t="s">
-        <v>275</v>
+        <v>262</v>
       </c>
       <c r="P17" s="33" t="s">
         <v>55</v>
@@ -4047,7 +4053,7 @@
         <v>55</v>
       </c>
       <c r="S17" s="33" t="s">
-        <v>285</v>
+        <v>272</v>
       </c>
       <c r="T17" s="33" t="s">
         <v>118</v>
@@ -4092,7 +4098,7 @@
         <v>55</v>
       </c>
       <c r="O18" s="33" t="s">
-        <v>276</v>
+        <v>263</v>
       </c>
       <c r="P18" s="33" t="s">
         <v>55</v>
@@ -4104,7 +4110,7 @@
         <v>55</v>
       </c>
       <c r="S18" s="33" t="s">
-        <v>285</v>
+        <v>272</v>
       </c>
       <c r="T18" s="33" t="s">
         <v>118</v>
@@ -4151,7 +4157,7 @@
         <v>55</v>
       </c>
       <c r="O19" s="33" t="s">
-        <v>276</v>
+        <v>263</v>
       </c>
       <c r="P19" s="33" t="s">
         <v>55</v>
@@ -4163,7 +4169,7 @@
         <v>55</v>
       </c>
       <c r="S19" s="33" t="s">
-        <v>285</v>
+        <v>272</v>
       </c>
       <c r="T19" s="33" t="s">
         <v>118</v>
@@ -4196,13 +4202,13 @@
         <v>45561</v>
       </c>
       <c r="G20" s="32" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="H20" s="32" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="I20" s="32" t="s">
-        <v>248</v>
+        <v>237</v>
       </c>
       <c r="J20" s="33" t="s">
         <v>55</v>
@@ -4216,7 +4222,7 @@
         <v>55</v>
       </c>
       <c r="O20" s="33" t="s">
-        <v>277</v>
+        <v>264</v>
       </c>
       <c r="P20" s="33" t="s">
         <v>55</v>
@@ -4228,7 +4234,7 @@
         <v>55</v>
       </c>
       <c r="S20" s="33" t="s">
-        <v>285</v>
+        <v>272</v>
       </c>
       <c r="T20" s="33" t="s">
         <v>118</v>
@@ -4259,13 +4265,13 @@
         <v>45561</v>
       </c>
       <c r="G21" s="32" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="H21" s="32" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="I21" s="32" t="s">
-        <v>249</v>
+        <v>238</v>
       </c>
       <c r="J21" s="33" t="s">
         <v>55</v>
@@ -4279,7 +4285,7 @@
         <v>55</v>
       </c>
       <c r="O21" s="33" t="s">
-        <v>278</v>
+        <v>265</v>
       </c>
       <c r="P21" s="33" t="s">
         <v>55</v>
@@ -4291,7 +4297,7 @@
         <v>55</v>
       </c>
       <c r="S21" s="33" t="s">
-        <v>285</v>
+        <v>272</v>
       </c>
       <c r="T21" s="33" t="s">
         <v>118</v>
@@ -4322,13 +4328,13 @@
         <v>45561</v>
       </c>
       <c r="G22" s="32" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="H22" s="32" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="I22" s="32" t="s">
-        <v>250</v>
+        <v>239</v>
       </c>
       <c r="J22" s="33" t="s">
         <v>55</v>
@@ -4342,7 +4348,7 @@
         <v>55</v>
       </c>
       <c r="O22" s="33" t="s">
-        <v>279</v>
+        <v>266</v>
       </c>
       <c r="P22" s="33" t="s">
         <v>55</v>
@@ -4354,7 +4360,7 @@
         <v>55</v>
       </c>
       <c r="S22" s="33" t="s">
-        <v>285</v>
+        <v>272</v>
       </c>
       <c r="T22" s="33" t="s">
         <v>118</v>
@@ -4385,13 +4391,13 @@
         <v>45561</v>
       </c>
       <c r="G23" s="32" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H23" s="32" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
       <c r="I23" s="32" t="s">
-        <v>251</v>
+        <v>240</v>
       </c>
       <c r="J23" s="33" t="s">
         <v>55</v>
@@ -4405,7 +4411,7 @@
         <v>55</v>
       </c>
       <c r="O23" s="33" t="s">
-        <v>280</v>
+        <v>267</v>
       </c>
       <c r="P23" s="33" t="s">
         <v>55</v>
@@ -4417,7 +4423,7 @@
         <v>55</v>
       </c>
       <c r="S23" s="33" t="s">
-        <v>285</v>
+        <v>272</v>
       </c>
       <c r="T23" s="33" t="s">
         <v>118</v>
@@ -4448,13 +4454,13 @@
         <v>45561</v>
       </c>
       <c r="G24" s="32" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="H24" s="32" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="I24" s="32" t="s">
-        <v>252</v>
+        <v>241</v>
       </c>
       <c r="J24" s="33" t="s">
         <v>55</v>
@@ -4468,7 +4474,7 @@
         <v>55</v>
       </c>
       <c r="O24" s="33" t="s">
-        <v>281</v>
+        <v>268</v>
       </c>
       <c r="P24" s="33" t="s">
         <v>55</v>
@@ -4480,7 +4486,7 @@
         <v>55</v>
       </c>
       <c r="S24" s="33" t="s">
-        <v>285</v>
+        <v>272</v>
       </c>
       <c r="T24" s="33" t="s">
         <v>118</v>
@@ -4511,13 +4517,13 @@
         <v>45561</v>
       </c>
       <c r="G25" s="32" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="H25" s="32" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="I25" s="32" t="s">
-        <v>253</v>
+        <v>242</v>
       </c>
       <c r="J25" s="33" t="s">
         <v>55</v>
@@ -4531,7 +4537,7 @@
         <v>55</v>
       </c>
       <c r="O25" s="33" t="s">
-        <v>282</v>
+        <v>269</v>
       </c>
       <c r="P25" s="33" t="s">
         <v>55</v>
@@ -4543,7 +4549,7 @@
         <v>55</v>
       </c>
       <c r="S25" s="33" t="s">
-        <v>285</v>
+        <v>272</v>
       </c>
       <c r="T25" s="33" t="s">
         <v>118</v>
@@ -4574,13 +4580,13 @@
         <v>45561</v>
       </c>
       <c r="G26" s="32" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="H26" s="32" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
       <c r="I26" s="32" t="s">
-        <v>254</v>
+        <v>243</v>
       </c>
       <c r="J26" s="33" t="s">
         <v>55</v>
@@ -4594,7 +4600,7 @@
         <v>55</v>
       </c>
       <c r="O26" s="33" t="s">
-        <v>283</v>
+        <v>270</v>
       </c>
       <c r="P26" s="33" t="s">
         <v>55</v>
@@ -4606,7 +4612,7 @@
         <v>55</v>
       </c>
       <c r="S26" s="33" t="s">
-        <v>286</v>
+        <v>273</v>
       </c>
       <c r="T26" s="33" t="s">
         <v>118</v>
@@ -4637,13 +4643,13 @@
         <v>45561</v>
       </c>
       <c r="G27" s="32" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="H27" s="32" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="I27" s="32" t="s">
-        <v>255</v>
+        <v>244</v>
       </c>
       <c r="J27" s="33" t="s">
         <v>55</v>
@@ -4657,7 +4663,7 @@
         <v>55</v>
       </c>
       <c r="O27" s="33" t="s">
-        <v>284</v>
+        <v>271</v>
       </c>
       <c r="P27" s="33" t="s">
         <v>55</v>
@@ -4669,7 +4675,7 @@
         <v>55</v>
       </c>
       <c r="S27" s="33" t="s">
-        <v>286</v>
+        <v>273</v>
       </c>
       <c r="T27" s="33" t="s">
         <v>118</v>
@@ -4782,13 +4788,13 @@
         <v>45561</v>
       </c>
       <c r="G30" s="32" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="H30" s="32" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
       <c r="I30" s="32" t="s">
-        <v>256</v>
+        <v>245</v>
       </c>
       <c r="J30" s="33" t="s">
         <v>55</v>
@@ -4802,7 +4808,7 @@
         <v>55</v>
       </c>
       <c r="O30" s="33" t="s">
-        <v>287</v>
+        <v>274</v>
       </c>
       <c r="P30" s="33" t="s">
         <v>55</v>
@@ -4814,7 +4820,7 @@
         <v>55</v>
       </c>
       <c r="S30" s="33" t="s">
-        <v>286</v>
+        <v>273</v>
       </c>
       <c r="T30" s="33" t="s">
         <v>118</v>
@@ -5050,13 +5056,13 @@
         <v>45561</v>
       </c>
       <c r="G36" s="32" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="H36" s="32" t="s">
-        <v>230</v>
+        <v>221</v>
       </c>
       <c r="I36" s="32" t="s">
-        <v>257</v>
+        <v>246</v>
       </c>
       <c r="J36" s="33" t="s">
         <v>55</v>
@@ -5070,7 +5076,7 @@
         <v>55</v>
       </c>
       <c r="O36" s="43" t="s">
-        <v>288</v>
+        <v>275</v>
       </c>
       <c r="P36" s="33" t="s">
         <v>55</v>
@@ -5082,7 +5088,7 @@
         <v>55</v>
       </c>
       <c r="S36" s="33" t="s">
-        <v>285</v>
+        <v>272</v>
       </c>
       <c r="T36" s="33" t="s">
         <v>118</v>
@@ -5113,13 +5119,13 @@
         <v>45561</v>
       </c>
       <c r="G37" s="32" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="H37" s="32" t="s">
-        <v>231</v>
+        <v>222</v>
       </c>
       <c r="I37" s="32" t="s">
-        <v>258</v>
+        <v>247</v>
       </c>
       <c r="J37" s="33" t="s">
         <v>55</v>
@@ -5133,7 +5139,7 @@
         <v>55</v>
       </c>
       <c r="O37" s="43" t="s">
-        <v>289</v>
+        <v>276</v>
       </c>
       <c r="P37" s="33" t="s">
         <v>55</v>
@@ -5145,7 +5151,7 @@
         <v>55</v>
       </c>
       <c r="S37" s="33" t="s">
-        <v>285</v>
+        <v>272</v>
       </c>
       <c r="T37" s="33" t="s">
         <v>118</v>
@@ -5176,13 +5182,13 @@
         <v>45561</v>
       </c>
       <c r="G38" s="32" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="H38" s="32" t="s">
-        <v>232</v>
+        <v>223</v>
       </c>
       <c r="I38" s="32" t="s">
-        <v>259</v>
+        <v>248</v>
       </c>
       <c r="J38" s="33" t="s">
         <v>55</v>
@@ -5196,7 +5202,7 @@
         <v>55</v>
       </c>
       <c r="O38" s="43" t="s">
-        <v>290</v>
+        <v>277</v>
       </c>
       <c r="P38" s="33" t="s">
         <v>55</v>
@@ -5208,7 +5214,7 @@
         <v>55</v>
       </c>
       <c r="S38" s="33" t="s">
-        <v>285</v>
+        <v>272</v>
       </c>
       <c r="T38" s="33" t="s">
         <v>118</v>
@@ -5239,13 +5245,13 @@
         <v>45561</v>
       </c>
       <c r="G39" s="32" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="H39" s="32" t="s">
-        <v>233</v>
+        <v>224</v>
       </c>
       <c r="I39" s="32" t="s">
-        <v>260</v>
+        <v>249</v>
       </c>
       <c r="J39" s="33" t="s">
         <v>55</v>
@@ -5259,7 +5265,7 @@
         <v>55</v>
       </c>
       <c r="O39" s="43" t="s">
-        <v>291</v>
+        <v>278</v>
       </c>
       <c r="P39" s="33" t="s">
         <v>55</v>
@@ -5271,7 +5277,7 @@
         <v>55</v>
       </c>
       <c r="S39" s="33" t="s">
-        <v>285</v>
+        <v>272</v>
       </c>
       <c r="T39" s="33" t="s">
         <v>118</v>
@@ -5302,13 +5308,13 @@
         <v>45561</v>
       </c>
       <c r="G40" s="32" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="H40" s="32" t="s">
-        <v>234</v>
+        <v>225</v>
       </c>
       <c r="I40" s="32" t="s">
-        <v>261</v>
+        <v>250</v>
       </c>
       <c r="J40" s="33" t="s">
         <v>55</v>
@@ -5322,7 +5328,7 @@
         <v>55</v>
       </c>
       <c r="O40" s="43" t="s">
-        <v>292</v>
+        <v>279</v>
       </c>
       <c r="P40" s="33" t="s">
         <v>55</v>
@@ -5334,7 +5340,7 @@
         <v>55</v>
       </c>
       <c r="S40" s="33" t="s">
-        <v>285</v>
+        <v>272</v>
       </c>
       <c r="T40" s="33" t="s">
         <v>118</v>
@@ -5365,13 +5371,13 @@
         <v>45561</v>
       </c>
       <c r="G41" s="32" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="H41" s="32" t="s">
-        <v>235</v>
+        <v>226</v>
       </c>
       <c r="I41" s="32" t="s">
-        <v>262</v>
+        <v>251</v>
       </c>
       <c r="J41" s="33" t="s">
         <v>55</v>
@@ -5385,7 +5391,7 @@
         <v>55</v>
       </c>
       <c r="O41" s="43" t="s">
-        <v>293</v>
+        <v>280</v>
       </c>
       <c r="P41" s="33" t="s">
         <v>55</v>
@@ -5397,7 +5403,7 @@
         <v>55</v>
       </c>
       <c r="S41" s="33" t="s">
-        <v>285</v>
+        <v>272</v>
       </c>
       <c r="T41" s="33" t="s">
         <v>118</v>
@@ -5428,13 +5434,13 @@
         <v>45561</v>
       </c>
       <c r="G42" s="32" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="H42" s="32" t="s">
-        <v>236</v>
+        <v>227</v>
       </c>
       <c r="I42" s="32" t="s">
-        <v>263</v>
+        <v>252</v>
       </c>
       <c r="J42" s="33" t="s">
         <v>55</v>
@@ -5448,7 +5454,7 @@
         <v>55</v>
       </c>
       <c r="O42" s="43" t="s">
-        <v>294</v>
+        <v>281</v>
       </c>
       <c r="P42" s="33" t="s">
         <v>55</v>
@@ -5460,7 +5466,7 @@
         <v>55</v>
       </c>
       <c r="S42" s="33" t="s">
-        <v>285</v>
+        <v>272</v>
       </c>
       <c r="T42" s="33" t="s">
         <v>118</v>
@@ -5491,13 +5497,13 @@
         <v>45561</v>
       </c>
       <c r="G43" s="32" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="H43" s="32" t="s">
-        <v>237</v>
+        <v>228</v>
       </c>
       <c r="I43" s="32" t="s">
-        <v>264</v>
+        <v>253</v>
       </c>
       <c r="J43" s="33" t="s">
         <v>55</v>
@@ -5511,7 +5517,7 @@
         <v>55</v>
       </c>
       <c r="O43" s="43" t="s">
-        <v>295</v>
+        <v>282</v>
       </c>
       <c r="P43" s="33" t="s">
         <v>55</v>
@@ -5523,7 +5529,7 @@
         <v>55</v>
       </c>
       <c r="S43" s="33" t="s">
-        <v>285</v>
+        <v>272</v>
       </c>
       <c r="T43" s="33" t="s">
         <v>118</v>
@@ -5554,13 +5560,13 @@
         <v>45561</v>
       </c>
       <c r="G44" s="32" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="H44" s="32" t="s">
-        <v>238</v>
+        <v>229</v>
       </c>
       <c r="I44" s="32" t="s">
-        <v>265</v>
+        <v>254</v>
       </c>
       <c r="J44" s="33" t="s">
         <v>55</v>
@@ -5574,7 +5580,7 @@
         <v>55</v>
       </c>
       <c r="O44" s="43" t="s">
-        <v>296</v>
+        <v>283</v>
       </c>
       <c r="P44" s="33" t="s">
         <v>55</v>
@@ -5586,7 +5592,7 @@
         <v>55</v>
       </c>
       <c r="S44" s="33" t="s">
-        <v>285</v>
+        <v>272</v>
       </c>
       <c r="T44" s="33" t="s">
         <v>118</v>
@@ -5617,13 +5623,13 @@
         <v>45561</v>
       </c>
       <c r="G45" s="32" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="H45" s="32" t="s">
-        <v>239</v>
+        <v>230</v>
       </c>
       <c r="I45" s="32" t="s">
-        <v>266</v>
+        <v>255</v>
       </c>
       <c r="J45" s="33" t="s">
         <v>55</v>
@@ -5637,7 +5643,7 @@
         <v>55</v>
       </c>
       <c r="O45" s="43" t="s">
-        <v>297</v>
+        <v>284</v>
       </c>
       <c r="P45" s="33" t="s">
         <v>55</v>
@@ -5649,7 +5655,7 @@
         <v>55</v>
       </c>
       <c r="S45" s="33" t="s">
-        <v>285</v>
+        <v>272</v>
       </c>
       <c r="T45" s="33" t="s">
         <v>118</v>
@@ -5680,13 +5686,13 @@
         <v>45561</v>
       </c>
       <c r="G46" s="32" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="H46" s="32" t="s">
-        <v>240</v>
+        <v>231</v>
       </c>
       <c r="I46" s="32" t="s">
-        <v>267</v>
+        <v>256</v>
       </c>
       <c r="J46" s="33" t="s">
         <v>55</v>
@@ -5700,7 +5706,7 @@
         <v>55</v>
       </c>
       <c r="O46" s="43" t="s">
-        <v>298</v>
+        <v>285</v>
       </c>
       <c r="P46" s="33" t="s">
         <v>55</v>
@@ -5712,7 +5718,7 @@
         <v>55</v>
       </c>
       <c r="S46" s="33" t="s">
-        <v>285</v>
+        <v>272</v>
       </c>
       <c r="T46" s="33" t="s">
         <v>118</v>
@@ -5743,13 +5749,13 @@
         <v>45561</v>
       </c>
       <c r="G47" s="32" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="H47" s="32" t="s">
-        <v>241</v>
+        <v>232</v>
       </c>
       <c r="I47" s="32" t="s">
-        <v>268</v>
+        <v>257</v>
       </c>
       <c r="J47" s="33" t="s">
         <v>55</v>
@@ -5763,7 +5769,7 @@
         <v>55</v>
       </c>
       <c r="O47" s="43" t="s">
-        <v>299</v>
+        <v>286</v>
       </c>
       <c r="P47" s="33" t="s">
         <v>55</v>
@@ -5775,7 +5781,7 @@
         <v>55</v>
       </c>
       <c r="S47" s="33" t="s">
-        <v>285</v>
+        <v>272</v>
       </c>
       <c r="T47" s="33" t="s">
         <v>118</v>
@@ -5806,13 +5812,13 @@
         <v>45561</v>
       </c>
       <c r="G48" s="32" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="H48" s="32" t="s">
-        <v>242</v>
+        <v>233</v>
       </c>
       <c r="I48" s="32" t="s">
-        <v>269</v>
+        <v>258</v>
       </c>
       <c r="J48" s="33" t="s">
         <v>55</v>
@@ -5826,7 +5832,7 @@
         <v>55</v>
       </c>
       <c r="O48" s="43" t="s">
-        <v>300</v>
+        <v>287</v>
       </c>
       <c r="P48" s="33" t="s">
         <v>55</v>
@@ -5838,7 +5844,7 @@
         <v>55</v>
       </c>
       <c r="S48" s="33" t="s">
-        <v>285</v>
+        <v>272</v>
       </c>
       <c r="T48" s="33" t="s">
         <v>118</v>
@@ -6033,13 +6039,13 @@
         <v>45561</v>
       </c>
       <c r="G53" s="32" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="H53" s="32" t="s">
-        <v>243</v>
+        <v>234</v>
       </c>
       <c r="I53" s="32" t="s">
-        <v>270</v>
+        <v>259</v>
       </c>
       <c r="J53" s="33" t="s">
         <v>55</v>
@@ -6053,7 +6059,7 @@
         <v>55</v>
       </c>
       <c r="O53" s="43" t="s">
-        <v>301</v>
+        <v>288</v>
       </c>
       <c r="P53" s="33" t="s">
         <v>55</v>
@@ -6065,7 +6071,7 @@
         <v>55</v>
       </c>
       <c r="S53" s="33" t="s">
-        <v>285</v>
+        <v>272</v>
       </c>
       <c r="T53" s="33" t="s">
         <v>118</v>
@@ -6096,13 +6102,13 @@
         <v>45561</v>
       </c>
       <c r="G54" s="32" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="H54" s="32" t="s">
-        <v>244</v>
+        <v>235</v>
       </c>
       <c r="I54" s="32" t="s">
-        <v>271</v>
+        <v>260</v>
       </c>
       <c r="J54" s="33" t="s">
         <v>55</v>
@@ -6116,7 +6122,7 @@
         <v>55</v>
       </c>
       <c r="O54" s="43" t="s">
-        <v>302</v>
+        <v>289</v>
       </c>
       <c r="P54" s="33" t="s">
         <v>55</v>
@@ -6128,7 +6134,7 @@
         <v>55</v>
       </c>
       <c r="S54" s="33" t="s">
-        <v>285</v>
+        <v>272</v>
       </c>
       <c r="T54" s="33" t="s">
         <v>118</v>
@@ -6156,16 +6162,16 @@
         <v>182</v>
       </c>
       <c r="F55" s="31">
-        <v>45561</v>
+        <v>45586</v>
       </c>
       <c r="G55" s="32" t="s">
-        <v>184</v>
+        <v>297</v>
       </c>
       <c r="H55" s="32" t="s">
-        <v>215</v>
+        <v>298</v>
       </c>
       <c r="I55" s="32" t="s">
-        <v>245</v>
+        <v>299</v>
       </c>
       <c r="J55" s="33" t="s">
         <v>55</v>
@@ -6205,16 +6211,16 @@
         <v>183</v>
       </c>
       <c r="F56" s="31">
-        <v>45561</v>
+        <v>45586</v>
       </c>
       <c r="G56" s="32" t="s">
-        <v>185</v>
+        <v>304</v>
       </c>
       <c r="H56" s="32" t="s">
-        <v>272</v>
+        <v>305</v>
       </c>
       <c r="I56" s="32" t="s">
-        <v>273</v>
+        <v>306</v>
       </c>
       <c r="J56" s="33" t="s">
         <v>55</v>
@@ -13109,27 +13115,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <UserStoryALM xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A92AB09DCDF6014AA0D6826BF29E2C8E" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d4db60622090a1f8a8d506ac1d64a349">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1e76d14e-d0ce-457c-8343-9b55836d9ead" xmlns:ns3="a56712a3-8dfd-4688-917a-22f0cf513b89" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0a3a9ed8bb952a3d76dd1e2fa3d624b9" ns2:_="" ns3:_="">
     <xsd:import namespace="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
@@ -13387,7 +13372,47 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <UserStoryALM xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{188DA7F5-158B-4F2F-BE68-E8B30B468193}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
+    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C4C806F-EC4E-4231-9462-6D32094C4603}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -13404,29 +13429,10 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{188DA7F5-158B-4F2F-BE68-E8B30B468193}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
-    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>